<commit_message>
added excel fetch data
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/User/CustomerDate.xlsx
+++ b/Group14-A2/src/main/java/User/CustomerDate.xlsx
@@ -1,13 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\javafx-restaurant-app\Group14-A2\src\main\java\User\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A906A8-93DE-483B-939D-BBA4F61C91C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="User Data" r:id="rId3" sheetId="1"/>
+    <sheet name="User Data" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -41,11 +49,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -57,7 +64,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -75,25 +82,335 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="7.578125" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.53515625" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.7421875" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.4375" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.203125" collapsed="false"/>
+    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -110,9 +427,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1.0</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -127,9 +444,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2.0</v>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -145,6 +462,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor: Refactoring code and adding some booleans and get and set methods
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/User/CustomerDate.xlsx
+++ b/Group14-A2/src/main/java/User/CustomerDate.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\javafx-restaurant-app\Group14-A2\src\main\java\User\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A906A8-93DE-483B-939D-BBA4F61C91C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B96E91-BE25-4949-8E7E-1ECF7EB98E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="1872" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>User ID</t>
   </si>
@@ -44,12 +44,25 @@
   </si>
   <si>
     <t>mmm@gmail.com</t>
+  </si>
+  <si>
+    <t>sauravsuresh171@gmail.com</t>
+  </si>
+  <si>
+    <t>Saurav</t>
+  </si>
+  <si>
+    <t>Suresh</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -395,19 +408,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="A4" sqref="A4:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.578125" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="27.38671875" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.7421875" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.4375" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.5078125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -461,6 +474,23 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feature : added feature to get the active customer in the customer landing page
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/User/CustomerDate.xlsx
+++ b/Group14-A2/src/main/java/User/CustomerDate.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>User ID</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>ss</t>
+  </si>
+  <si>
+    <t>sursau@outlook.com</t>
   </si>
 </sst>
 </file>
@@ -98,18 +101,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="7.578125" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="27.38671875" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.7421875" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.4375" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.203125" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9.98828125" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="27.38671875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.7421875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.4375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.203125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="9.98828125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -172,6 +175,26 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
added the model box along with the buttons and ui
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/User/CustomerDate.xlsx
+++ b/Group14-A2/src/main/java/User/CustomerDate.xlsx
@@ -1,18 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\javafx-restaurant-app\Group14-A2\src\main\java\User\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02C7C26-C498-459F-A861-44BCB1FF352F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="User Data" r:id="rId3" sheetId="1"/>
+    <sheet name="User Data" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>User ID</t>
   </si>
@@ -54,19 +62,15 @@
   </si>
   <si>
     <t>ss</t>
-  </si>
-  <si>
-    <t>sursau@outlook.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -78,7 +82,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -96,26 +100,336 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="7.578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="27.38671875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.7421875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.4375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.203125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9.98828125" collapsed="true"/>
+    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -135,9 +449,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1.0</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -155,9 +469,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2.0</v>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -175,12 +489,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3.0</v>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -196,6 +510,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added code for staff user create
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/User/CustomerDate.xlsx
+++ b/Group14-A2/src/main/java/User/CustomerDate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\javafx-restaurant-app\Group14-A2\src\main\java\User\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02C7C26-C498-459F-A861-44BCB1FF352F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDA1B6F-5DC8-4DFE-99BD-E8E6C7A116F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -416,7 +416,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -451,7 +451,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -471,7 +471,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -491,7 +491,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
added jdocs and fixed issue with user create email regex check
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/User/CustomerDate.xlsx
+++ b/Group14-A2/src/main/java/User/CustomerDate.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\javafx-restaurant-app\Group14-A2\src\main\java\User\"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>User ID</t>
   </si>
@@ -62,12 +62,16 @@
   </si>
   <si>
     <t>ss</t>
+  </si>
+  <si>
+    <t>testuser@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -413,7 +417,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -421,12 +425,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="27.38671875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.7421875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.4375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.203125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="9.98828125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -509,6 +513,26 @@
         <v>10</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor : Main file
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/User/CustomerDate.xlsx
+++ b/Group14-A2/src/main/java/User/CustomerDate.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\javafx-restaurant-app\Group14-A2\src\main\java\User\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDA1B6F-5DC8-4DFE-99BD-E8E6C7A116F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9713E19D-C325-46C7-BAC8-DC894CA7E328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="852" yWindow="2424" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Data" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -441,17 +440,17 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="7.578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="27.38671875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.7421875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.4375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="26.6484375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9.98828125" collapsed="true"/>
+    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -534,9 +533,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>9.0</v>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -554,9 +553,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>10.0</v>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -574,9 +573,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>16.0</v>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
@@ -594,9 +593,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>18.0</v>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>

</xml_diff>